<commit_message>
Finished with project 4!
</commit_message>
<xml_diff>
--- a/ece-18-642/lec-10-to-14/proj04/peer_review_Nguyen_Todd_noid.xlsx
+++ b/ece-18-642/lec-10-to-14/proj04/peer_review_Nguyen_Todd_noid.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Peer Review Checklist   18-642</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>Time spent:</t>
+  </si>
+  <si>
+    <t>Thursday May 18, 2021</t>
+  </si>
+  <si>
+    <t>Project 3 source code</t>
+  </si>
+  <si>
+    <t>Todd Nguyen</t>
+  </si>
+  <si>
+    <t>Lack of comment on each function. However, the function name might be more than enough for a comment.</t>
+  </si>
+  <si>
+    <t>Not a Bug</t>
+  </si>
+  <si>
+    <t>Some structs can be typedef.</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
   </si>
 </sst>
 </file>
@@ -119,11 +140,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -132,6 +150,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -512,146 +542,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>1</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="2">
         <v>2</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="2">
         <v>3</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="2">
         <v>4</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="2">
         <v>5</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="2">
         <v>6</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="2">
         <v>7</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="2">
         <v>8</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="2">
         <v>9</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="2">
         <v>10</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="2">
         <v>11</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="2">
         <v>12</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="2">
         <v>13</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="2">
         <v>14</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="2">
         <v>15</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">

</xml_diff>